<commit_message>
try 95 to 50 percentile 200 tags
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFC3607-6C2A-DB43-95D1-5481C3E41DBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4E2359-6AC3-B742-B4E7-B9D423A9107C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="14900" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
+    <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Synopsis_tag_embeddings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Model Version</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Softmax activation with categorical cross entropy loss</t>
   </si>
   <si>
-    <t>metadata_dev_edc_base_0_0_3_20210422213203</t>
-  </si>
-  <si>
     <t>Setup</t>
   </si>
   <si>
@@ -76,6 +73,36 @@
   </si>
   <si>
     <t>Sigmoid actiavtion with binary cross entropy loss, using edc data, 100 tags</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_3_20210423134837</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4</t>
+  </si>
+  <si>
+    <t>More hidden layers; my own data; train with binary cross-entropy</t>
+  </si>
+  <si>
+    <t>More hidden layers; my own data; train with cosine similarity</t>
+  </si>
+  <si>
+    <t>More hidden layers; Dylan data; train with binary cross-entropy</t>
+  </si>
+  <si>
+    <t>More hidden layers; Dylan data; train with cosine similarity</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210426235033</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210427024035</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210427025038</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210427034633</t>
   </si>
 </sst>
 </file>
@@ -128,8 +155,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -455,86 +483,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="114" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="29.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" location="/pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/a77848d3-ecce-4c1e-980b-e81464cf3922" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/a77848d3-ecce-4c1e-980b-e81464cf3922" xr:uid="{6CADB887-E914-A548-BD60-14E3B72B0825}"/>
     <hyperlink ref="B4" r:id="rId2" location="/pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/8749b116-3366-4768-bbc9-84655219119b" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/8749b116-3366-4768-bbc9-84655219119b" xr:uid="{4D8C4DBB-6579-EA45-8B22-D2EF85202988}"/>
-    <hyperlink ref="B5" r:id="rId3" location="/pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/46bedd5e-658d-47b2-bc12-9c9ee536526b" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/46bedd5e-658d-47b2-bc12-9c9ee536526b" xr:uid="{25D665A7-BB13-3049-A7B5-13B444240C8A}"/>
-    <hyperlink ref="B2" r:id="rId4" location="/pipelines/details/2d03a5e5-98f6-4227-8359-7df4434bba59/version/fa6e652e-b9b0-40dc-a4ad-9d5fc0847b36" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/2d03a5e5-98f6-4227-8359-7df4434bba59/version/fa6e652e-b9b0-40dc-a4ad-9d5fc0847b36" xr:uid="{039C9CF1-62DD-4F4B-883C-5A30A0D21833}"/>
+    <hyperlink ref="B2" r:id="rId3" location="/pipelines/details/2d03a5e5-98f6-4227-8359-7df4434bba59/version/fa6e652e-b9b0-40dc-a4ad-9d5fc0847b36" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/2d03a5e5-98f6-4227-8359-7df4434bba59/version/fa6e652e-b9b0-40dc-a4ad-9d5fc0847b36" xr:uid="{039C9CF1-62DD-4F4B-883C-5A30A0D21833}"/>
+    <hyperlink ref="B5" r:id="rId4" location="/pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/b83837ad-21ec-4b02-883a-adde0a4ac481" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/b83837ad-21ec-4b02-883a-adde0a4ac481" xr:uid="{4B99E3D9-13DC-3844-9693-8F849FAAE0C1}"/>
+    <hyperlink ref="B6" r:id="rId5" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/886039c0-854f-41eb-93a2-bb207ca38627" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/886039c0-854f-41eb-93a2-bb207ca38627" xr:uid="{BE451817-B1C2-484D-9159-FBE548FAAB28}"/>
+    <hyperlink ref="B7" r:id="rId6" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0f8ad371-21aa-4938-bf60-984f0b06c079" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0f8ad371-21aa-4938-bf60-984f0b06c079" xr:uid="{2ACC4C89-1A2A-304C-A9E1-7F526EC13E5F}"/>
+    <hyperlink ref="B8" r:id="rId7" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/4f1ad934-d906-44e7-9fe2-7bf0c1817de1" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/4f1ad934-d906-44e7-9fe2-7bf0c1817de1" xr:uid="{F48B702F-8538-2145-A364-4423DF860EAC}"/>
+    <hyperlink ref="B9" r:id="rId8" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5106c84f-991f-4146-867e-cc3d76eb0813" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5106c84f-991f-4146-867e-cc3d76eb0813" xr:uid="{5513A0CA-55BE-3E48-BEC4-C38D78FC1216}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
try dylan data with token
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4E2359-6AC3-B742-B4E7-B9D423A9107C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1434AE8-74BA-4249-A105-B1AA5E1DB7B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Synopsis_tag_embeddings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Model Version</t>
   </si>
@@ -103,13 +103,120 @@
   </si>
   <si>
     <t>metadata_dev_edc_base_0_0_4_20210427034633</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210427142856</t>
+  </si>
+  <si>
+    <t>More hidden layers; my own data with now 200 labels instead of 100; train with binary cross-entropy</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210428014009</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210428010543</t>
+  </si>
+  <si>
+    <t>No hidden layers; my own data with node2vec tokens; train with binary cross entropy.</t>
+  </si>
+  <si>
+    <t>With Hidden layers; only 20 rows of data; now with additional node2vec tokens extracted from synopsis. inference time can perform tomorrow. If that does not help, then the evaluation step very likely have a problem</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>INSIGHT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: However, the item-to-item recs on each user had similar performance comparing using the full data training. Implications: either the script to do evaluation is wrong, or the averaging is drowning out anything useful learned in the embeddings. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>TODO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Ask Dylan how well setting the known tags to 1 at</t>
+    </r>
+  </si>
+  <si>
+    <t>Do another experiment here: With Dylan's data, without tokens, limit 20 to train, eval on the full set. See how well it performs against exp row 5</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.0128
+Precision@5 : 0.011407999999999849
+Precision@10 : 0.010844000000000886
+Recall@1 : 0.0026346666666666875
+Recall@5 : 0.011657666666666544
+Recall@10 : 0.02215633333333501
+Accuracy@1 : 0.0128
+Accuracy@5 : 0.055
+Accuracy@10 : 0.0997
+Coverage@1 : 0.3940236275191105
+Coverage@5 : 0.6268241834607367
+Coverage@10 : 0.753995830437804</t>
+  </si>
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.0089
+Precision@5 : 0.00824399999999971
+Precision@10 : 0.007698000000000317
+Recall@1 : 0.0018000000000000134
+Recall@5 : 0.008439333333333052
+Recall@10 : 0.01572900000000058
+Accuracy@1 : 0.0089
+Accuracy@5 : 0.04032
+Accuracy@10 : 0.07306
+Coverage@1 : 0.23314993122420907
+Coverage@5 : 0.391334250343879
+Coverage@10 : 0.49449793672627235</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.00916
+Precision@5 : 0.008803999999999684
+Precision@10 : 0.008322000000000435
+Recall@1 : 0.0019260000000000139
+Recall@5 : 0.009087999999999695
+Recall@10 : 0.017074333333334156
+Accuracy@1 : 0.00916
+Accuracy@5 : 0.04292
+Accuracy@10 : 0.07928
+Coverage@1 : 0.406721536351166
+Coverage@5 : 0.635116598079561
+Coverage@10 : 0.7578875171467764</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,6 +239,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -483,22 +595,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="114" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="114" workbookViewId="0">
+      <selection activeCell="F7" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="43.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="51.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -511,8 +624,11 @@
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -524,7 +640,7 @@
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -535,7 +651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -546,7 +662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="204" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -556,8 +672,11 @@
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -567,8 +686,11 @@
       <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -579,7 +701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -590,7 +712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -599,6 +721,50 @@
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="C13" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -611,6 +777,9 @@
     <hyperlink ref="B7" r:id="rId6" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0f8ad371-21aa-4938-bf60-984f0b06c079" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0f8ad371-21aa-4938-bf60-984f0b06c079" xr:uid="{2ACC4C89-1A2A-304C-A9E1-7F526EC13E5F}"/>
     <hyperlink ref="B8" r:id="rId7" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/4f1ad934-d906-44e7-9fe2-7bf0c1817de1" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/4f1ad934-d906-44e7-9fe2-7bf0c1817de1" xr:uid="{F48B702F-8538-2145-A364-4423DF860EAC}"/>
     <hyperlink ref="B9" r:id="rId8" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5106c84f-991f-4146-867e-cc3d76eb0813" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5106c84f-991f-4146-867e-cc3d76eb0813" xr:uid="{5513A0CA-55BE-3E48-BEC4-C38D78FC1216}"/>
+    <hyperlink ref="B10" r:id="rId9" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/18e914b3-fabc-43ed-bf9b-53004e624a6f" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/18e914b3-fabc-43ed-bf9b-53004e624a6f" xr:uid="{58D3158F-006A-F146-B3B5-8741FD236400}"/>
+    <hyperlink ref="B12" r:id="rId10" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/f013bd7f-c122-4130-9817-733ed0251dd5" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/f013bd7f-c122-4130-9817-733ed0251dd5" xr:uid="{8D46A18F-6877-FD49-9F74-C1A476B1E63E}"/>
+    <hyperlink ref="B11" r:id="rId11" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9ae49c61-0512-4ae3-ab82-aaf630837157" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9ae49c61-0512-4ae3-ab82-aaf630837157" xr:uid="{BAA3A710-C9BA-944B-A594-F9E4859C8A28}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
try reduced data on eval
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1434AE8-74BA-4249-A105-B1AA5E1DB7B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724825C9-9294-F147-83F2-2E38CC75D19A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
+    <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Synopsis_tag_embeddings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>Model Version</t>
   </si>
@@ -164,9 +164,6 @@
     </r>
   </si>
   <si>
-    <t>Do another experiment here: With Dylan's data, without tokens, limit 20 to train, eval on the full set. See how well it performs against exp row 5</t>
-  </si>
-  <si>
     <t>Precision@1 : 0.0128
 Precision@5 : 0.011407999999999849
 Precision@10 : 0.010844000000000886
@@ -210,6 +207,55 @@
 Coverage@1 : 0.406721536351166
 Coverage@5 : 0.635116598079561
 Coverage@10 : 0.7578875171467764</t>
+  </si>
+  <si>
+    <t>No hidden layers; Dylans data with node2vec tokens, train with binary cross entropy</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.01186
+Precision@5 : 0.010879999999999737
+Precision@10 : 0.009896000000000736
+Recall@1 : 0.002425333333333355
+Recall@5 : 0.011122999999999772
+Recall@10 : 0.020352000000001393
+Accuracy@1 : 0.01186
+Accuracy@5 : 0.05236
+Accuracy@10 : 0.09264
+Coverage@1 : 0.40646492434663
+Coverage@5 : 0.6464924346629987
+Coverage@10 : 0.7647867950481431</t>
+  </si>
+  <si>
+    <t>Dag link</t>
+  </si>
+  <si>
+    <t>https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/#/runs/details/f1163bd7-b8d4-445a-a42e-4edaf56e8d9f</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.0164
+Precision@5 : 0.014508000000000411
+Precision@10 : 0.01325200000000131
+Recall@1 : 0.0034513333333333197
+Recall@5 : 0.015017666666667073
+Recall@10 : 0.027325333333335717
+Accuracy@1 : 0.0164
+Accuracy@5 : 0.06698
+Accuracy@10 : 0.11728
+Coverage@1 : 0.5166780122532335
+Coverage@5 : 0.773995915588836
+Coverage@10 : 0.8761061946902655</t>
+  </si>
+  <si>
+    <t>https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/#/runs/details/05d53fcc-72d4-4236-bdde-621a2fb04b0c</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210428023440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accuracy increased by ~2%, indicating this approach is helpful. In fact, all metrics were increased. </t>
+  </si>
+  <si>
+    <t>Do another experiment here: With Dylan's data, without tokens, limit 20 to train, eval on the full set. See how well it performs against exp row 5, and row 13</t>
   </si>
 </sst>
 </file>
@@ -595,176 +641,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="114" workbookViewId="0">
-      <selection activeCell="F7" sqref="F6:F7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="114" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="43.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="51.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="39.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="13.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+      <c r="F5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F11" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C13" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -780,6 +869,7 @@
     <hyperlink ref="B10" r:id="rId9" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/18e914b3-fabc-43ed-bf9b-53004e624a6f" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/18e914b3-fabc-43ed-bf9b-53004e624a6f" xr:uid="{58D3158F-006A-F146-B3B5-8741FD236400}"/>
     <hyperlink ref="B12" r:id="rId10" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/f013bd7f-c122-4130-9817-733ed0251dd5" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/f013bd7f-c122-4130-9817-733ed0251dd5" xr:uid="{8D46A18F-6877-FD49-9F74-C1A476B1E63E}"/>
     <hyperlink ref="B11" r:id="rId11" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9ae49c61-0512-4ae3-ab82-aaf630837157" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9ae49c61-0512-4ae3-ab82-aaf630837157" xr:uid="{BAA3A710-C9BA-944B-A594-F9E4859C8A28}"/>
+    <hyperlink ref="B13" r:id="rId12" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/8d0e5341-e919-4d22-bb9d-5a235f635c29" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/8d0e5341-e919-4d22-bb9d-5a235f635c29" xr:uid="{C852A73B-8BFA-FB4C-8C90-A66826250654}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
using keywords only focal loss
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353203D6-77CE-7F42-8798-F640C752FA4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F75363-E110-C44B-AAD5-9C5CEFBBD50A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>Model Version</t>
   </si>
@@ -341,6 +341,12 @@
 Coverage@1 0.31239804241435565
 Coverage@5 0.4893964110929853
 Coverage@10 0.6092985318107668</t>
+  </si>
+  <si>
+    <t>No hidden layers; Dylans data with node2vec tokens, averaged embed vector repeated 4 times; train with focal loss default parameters gamma=2.0, alpha=0.25</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210428162402</t>
   </si>
 </sst>
 </file>
@@ -730,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="114" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -982,6 +988,17 @@
       </c>
       <c r="E18" s="3" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1006,6 +1023,8 @@
     <hyperlink ref="B16" r:id="rId18" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/beb3555c-3ca6-4dcb-a3ce-ce5d17db9deb" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/beb3555c-3ca6-4dcb-a3ce-ce5d17db9deb" xr:uid="{138789EA-3C7F-F043-8D4E-25DFD8597CA3}"/>
     <hyperlink ref="A17" r:id="rId19" location="/runs/details/7dc1fe4b-4048-40b5-aa4c-a2109ccc5446" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/7dc1fe4b-4048-40b5-aa4c-a2109ccc5446" xr:uid="{82CC4711-3C00-0A47-B528-F4D0AE38528A}"/>
     <hyperlink ref="B17" r:id="rId20" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5430845c-abf4-4986-950f-a7475c36debd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5430845c-abf4-4986-950f-a7475c36debd" xr:uid="{D822687D-B057-2649-9288-155ACA16B32F}"/>
+    <hyperlink ref="B19" r:id="rId21" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/491ce751-af86-4aa2-b8e6-b8a5c182593a" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/491ce751-af86-4aa2-b8e6-b8a5c182593a" xr:uid="{57618230-5285-324A-A1A4-3B3F11257C75}"/>
+    <hyperlink ref="A19" r:id="rId22" location="/runs/details/66f64249-e696-4c9d-94ad-55d4d6cca0bd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/66f64249-e696-4c9d-94ad-55d4d6cca0bd" xr:uid="{049A3D84-8C37-9A41-A40A-FDE3B5FEA125}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rerun on eval data
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F75363-E110-C44B-AAD5-9C5CEFBBD50A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817F9F7F-DB12-8940-992B-F0A9BA3D4AEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Synopsis_tag_embeddings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>Model Version</t>
   </si>
@@ -347,6 +347,49 @@
   </si>
   <si>
     <t>metadata_dev_edc_base_0_0_4_20210428162402</t>
+  </si>
+  <si>
+    <t>Significant gain of Accuracy@10</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.0208
+Precision@5 : 0.016764000000000844
+Precision@10 : 0.015066000000001661
+Recall@1 : 0.004268333333333274
+Recall@5 : 0.017234666666667463
+Recall@10 : 0.030954000000003038
+Accuracy@1 : 0.0208
+Accuracy@5 : 0.07742
+Accuracy@10 : 0.1318
+Coverage@1 : 0.4470827679782904
+Coverage@5 : 0.6879240162822252
+Coverage@10 : 0.8113975576662144</t>
+  </si>
+  <si>
+    <t>Didn’t add too much on the metrics</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.01422
+Precision@5 : 0.012932000000000147
+Precision@10 : 0.012272000000001126
+Recall@1 : 0.002922000000000008
+Recall@5 : 0.013272000000000141
+Recall@10 : 0.025181000000002077
+Accuracy@1 : 0.01422
+Accuracy@5 : 0.06068
+Accuracy@10 : 0.11046
+Coverage@1 : 0.35888738127544095
+Coverage@5 : 0.5746268656716418
+Coverage@10 : 0.6702849389416553</t>
+  </si>
+  <si>
+    <t>No hidden layers; Dylans data with node2vec tokens on Keywords; train with focal loss default parameters.</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210428202253</t>
+  </si>
+  <si>
+    <t>Using keywords only does not help</t>
   </si>
 </sst>
 </file>
@@ -736,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="114" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,11 +1029,14 @@
       <c r="C18" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E18" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="204" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -999,6 +1045,29 @@
       </c>
       <c r="C19" s="3" t="s">
         <v>53</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1025,6 +1094,8 @@
     <hyperlink ref="B17" r:id="rId20" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5430845c-abf4-4986-950f-a7475c36debd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5430845c-abf4-4986-950f-a7475c36debd" xr:uid="{D822687D-B057-2649-9288-155ACA16B32F}"/>
     <hyperlink ref="B19" r:id="rId21" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/491ce751-af86-4aa2-b8e6-b8a5c182593a" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/491ce751-af86-4aa2-b8e6-b8a5c182593a" xr:uid="{57618230-5285-324A-A1A4-3B3F11257C75}"/>
     <hyperlink ref="A19" r:id="rId22" location="/runs/details/66f64249-e696-4c9d-94ad-55d4d6cca0bd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/66f64249-e696-4c9d-94ad-55d4d6cca0bd" xr:uid="{049A3D84-8C37-9A41-A40A-FDE3B5FEA125}"/>
+    <hyperlink ref="A20" r:id="rId23" location="/runs/details/a397faf3-0a4a-4402-ad2d-2b9ae2cac042" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/a397faf3-0a4a-4402-ad2d-2b9ae2cac042" xr:uid="{E1FA6024-D942-6C47-8ACE-C1F35F13BC9C}"/>
+    <hyperlink ref="B20" r:id="rId24" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/3c628aad-f449-4ac5-8e13-6ace2595cf92" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/3c628aad-f449-4ac5-8e13-6ace2595cf92" xr:uid="{DFCFE686-61A9-9049-AF97-B2680FE4A4C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
try with alpha 0.75
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72A58CC-D969-C24D-A1C6-13053582A549}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6C6A80-C6BD-6F47-A727-2853FB849363}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
@@ -601,9 +601,6 @@
     <t>metadata_dev_edc_base_0_0_4_20210429160416</t>
   </si>
   <si>
-    <t>Correct mistake with "movies" tag. Rerun with gamma=3.0, alpha=0.25, full dataset from Dylan, with only keyword embeddings</t>
-  </si>
-  <si>
     <t>Alternative concatenation: at training time, feed only the bert output to the dense layer, but then at inference time, concatenate the token embeddings. Focal loss gamm=2.0, alpha=0.25</t>
   </si>
   <si>
@@ -621,13 +618,16 @@
 Coverage@10 : 0.8918187964841109</t>
   </si>
   <si>
-    <t>metadata_dev_edc_base_0_0_4_20210429174904</t>
-  </si>
-  <si>
     <t>Correct mistakes with "movie" tag. Rerun with gamma=3.0, alpha=0.25, full dataset from Dylan, with keyword embeddings concatenated only at prediction</t>
   </si>
   <si>
-    <t>metadata_dev_edc_base_0_0_4_20210429182108</t>
+    <t>metadata_dev_edc_base_0_0_4_20210429195106</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210429200232</t>
+  </si>
+  <si>
+    <t>Correct mistake with "movies" tag. Rerun with gamma=3.0, alpha=0.25, full dataset from Dylan, with only keyword embeddings concatenated before feeding into final dense layer</t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1457,10 +1457,10 @@
         <v>87</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1471,18 +1471,18 @@
         <v>91</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1570,10 +1570,10 @@
     <hyperlink ref="A27" r:id="rId36" location="/runs/details/fe703800-5ed4-48a7-8959-ca9cd00669a6" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/fe703800-5ed4-48a7-8959-ca9cd00669a6" xr:uid="{7C97D0F8-ECA2-744D-8D9C-81D113EA2772}"/>
     <hyperlink ref="A28" r:id="rId37" location="/runs/details/85ef22c4-3bfb-4c8a-abb0-6f5a7ef4bd3c" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/85ef22c4-3bfb-4c8a-abb0-6f5a7ef4bd3c" xr:uid="{74EF2AAC-46D5-8D47-BD77-DA5116E08B0D}"/>
     <hyperlink ref="B28" r:id="rId38" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9604be9a-0bc3-4f4b-b3fe-573c43c58614" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9604be9a-0bc3-4f4b-b3fe-573c43c58614" xr:uid="{00E298FB-22B7-5A45-8815-706BFE7141AD}"/>
-    <hyperlink ref="A29" r:id="rId39" location="/runs/details/88c2205b-f16e-4053-9121-eecde66ba0b8" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/88c2205b-f16e-4053-9121-eecde66ba0b8" xr:uid="{99A99E18-1C95-CA49-8D1D-E2051D9AF5BC}"/>
-    <hyperlink ref="B29" r:id="rId40" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/337359c6-9e9d-4e5e-b5b0-64b0df9f3629" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/337359c6-9e9d-4e5e-b5b0-64b0df9f3629" xr:uid="{3E94DB18-1AD9-C14D-85D9-0E64F5364CD9}"/>
-    <hyperlink ref="B30" r:id="rId41" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/435eaa1c-8bdf-4ac7-abde-d63c4ad618ac" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/435eaa1c-8bdf-4ac7-abde-d63c4ad618ac" xr:uid="{FF5618A1-7B84-2E4A-95DE-B189E8BC756D}"/>
-    <hyperlink ref="A30" r:id="rId42" location="/runs/details/a3b467b8-9fbc-4813-9a62-e1f424081d6c" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/a3b467b8-9fbc-4813-9a62-e1f424081d6c" xr:uid="{35468991-0378-4647-B190-EF9A9C0E6E2F}"/>
+    <hyperlink ref="A29" r:id="rId39" location="/runs/details/2173aac9-2fc6-41fa-be94-a81a105abe56" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/2173aac9-2fc6-41fa-be94-a81a105abe56" xr:uid="{F172878E-4B3A-2540-9138-C75A12D2E948}"/>
+    <hyperlink ref="B29" r:id="rId40" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/46949b0f-4756-4035-8bc3-18e961d85545" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/46949b0f-4756-4035-8bc3-18e961d85545" xr:uid="{33762F08-B4E2-EA40-AF59-D34CA2C37B89}"/>
+    <hyperlink ref="B30" r:id="rId41" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/618cb506-ab3b-40fd-b13a-c432466f5a55" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/618cb506-ab3b-40fd-b13a-c432466f5a55" xr:uid="{35066E55-C490-444F-90CF-EC8B6943ED77}"/>
+    <hyperlink ref="A30" r:id="rId42" location="/runs/details/0ece7dde-344b-4e1e-a84c-48075de44051" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/0ece7dde-344b-4e1e-a84c-48075de44051" xr:uid="{3828495F-E236-8448-A21D-54ADF5F1F67C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
alpha 0.75 concat after dense
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6C6A80-C6BD-6F47-A727-2853FB849363}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5B9D8D-8D30-214B-B175-03BF32880DC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="99">
   <si>
     <t>Model Version</t>
   </si>
@@ -628,6 +628,54 @@
   </si>
   <si>
     <t>Correct mistake with "movies" tag. Rerun with gamma=3.0, alpha=0.25, full dataset from Dylan, with only keyword embeddings concatenated before feeding into final dense layer</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.02924
+Precision@5 : 0.023600000000002175
+Precision@10 : 0.020392000000002776
+Recall@1 : 0.005915999999999841
+Recall@5 : 0.02383266666666877
+Recall@10 : 0.041191333333338555
+Accuracy@1 : 0.02924
+Accuracy@5 : 0.10826
+Accuracy@10 : 0.17732
+Coverage@1 : 0.5279085406859448
+Coverage@5 : 0.8069939475453934
+Coverage@10 : 0.9071956960322798</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.02528
+Precision@5 : 0.02164400000000167
+Precision@10 : 0.019158000000002465
+Recall@1 : 0.005131999999999887
+Recall@5 : 0.02187566666666831
+Recall@10 : 0.03872066666667147
+Accuracy@1 : 0.02528
+Accuracy@5 : 0.09856
+Accuracy@10 : 0.16404
+Coverage@1 : 0.5070611970410221
+Coverage@5 : 0.7646267652992602
+Coverage@10 : 0.8755884330867518</t>
+  </si>
+  <si>
+    <t>Rerun with gamma=3.0, alpha=0.75, full dataset from Dylan, with only keyword embeddings concatenated before feeding into final dense layer</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210429211642</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.02798
+Precision@5 : 0.023192000000002023
+Precision@10 : 0.020264000000002672
+Recall@1 : 0.0056486666666665224
+Recall@5 : 0.023419000000001966
+Recall@10 : 0.04094333333333853
+Accuracy@1 : 0.02798
+Accuracy@5 : 0.1049
+Accuracy@10 : 0.17192
+Coverage@1 : 0.47747141896435774
+Coverage@5 : 0.7753866845998655
+Coverage@10 : 0.8695359784801614</t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1459,11 +1507,11 @@
       <c r="C28" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
@@ -1473,8 +1521,11 @@
       <c r="C29" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="E29" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -1484,10 +1535,23 @@
       <c r="C30" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="E30" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -1574,6 +1638,8 @@
     <hyperlink ref="B29" r:id="rId40" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/46949b0f-4756-4035-8bc3-18e961d85545" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/46949b0f-4756-4035-8bc3-18e961d85545" xr:uid="{33762F08-B4E2-EA40-AF59-D34CA2C37B89}"/>
     <hyperlink ref="B30" r:id="rId41" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/618cb506-ab3b-40fd-b13a-c432466f5a55" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/618cb506-ab3b-40fd-b13a-c432466f5a55" xr:uid="{35066E55-C490-444F-90CF-EC8B6943ED77}"/>
     <hyperlink ref="A30" r:id="rId42" location="/runs/details/0ece7dde-344b-4e1e-a84c-48075de44051" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/0ece7dde-344b-4e1e-a84c-48075de44051" xr:uid="{3828495F-E236-8448-A21D-54ADF5F1F67C}"/>
+    <hyperlink ref="A31" r:id="rId43" location="/runs/details/9908e4bf-71ab-4f5b-8c7f-c4b374bf7a65" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/9908e4bf-71ab-4f5b-8c7f-c4b374bf7a65" xr:uid="{AED4D5B8-7808-3241-A1C4-108A980111D2}"/>
+    <hyperlink ref="B31" r:id="rId44" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/7cea8693-b60a-4622-a597-3d370feda18d" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/7cea8693-b60a-4622-a597-3d370feda18d" xr:uid="{A6960C78-B1EF-8B45-97D1-9076EC413127}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
try full set of tags
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5B9D8D-8D30-214B-B175-03BF32880DC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7F18D6-3C4B-BD44-ACAF-E6A921B2ADDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="114">
   <si>
     <t>Model Version</t>
   </si>
@@ -306,9 +306,6 @@
 Coverage@10 : 0.8181818181818182</t>
   </si>
   <si>
-    <t>Do another experiment here: With Dylan's data, without tokens, limit 20 to train, eval on the full set. See how well it performs against exp row 7, and row 15</t>
-  </si>
-  <si>
     <t>Benchmark raw tags and subgenres</t>
   </si>
   <si>
@@ -677,12 +674,168 @@
 Coverage@5 : 0.7753866845998655
 Coverage@10 : 0.8695359784801614</t>
   </si>
+  <si>
+    <t>Rerun with gamma=3.0, alpha=0.75, full dataset from Dylan, with only keyword embeddings concatenated after feeding bert output into final dense layer</t>
+  </si>
+  <si>
+    <t>INFO:absl:json_outputs='{"model": [{"artifact": {"id": "21208", "type_id": "16", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_4/Trainer/model/22706", "custom_properties": {"name": {"string_value": "model"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "16", "name": "Model"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "Model"}], "model_run": [{"artifact": {"id": "21209", "type_id": "17", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_4/Trainer/model_run/22706", "custom_properties": {"name": {"string_value": "model_run"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "17", "name": "ModelRun"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "ModelRun"}]}'.</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210429224329</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.03
+Precision@5 : 0.024452000000002354
+Precision@10 : 0.02106600000000236
+Recall@1 : 0.0060576666666665
+Recall@5 : 0.024704666666668935
+Recall@10 : 0.042569333333337775
+Accuracy@1 : 0.03
+Accuracy@5 : 0.1117
+Accuracy@10 : 0.18198
+Coverage@1 : 0.5151311365164761
+Coverage@5 : 0.7881640887693342
+Coverage@10 : 0.8863483523873571</t>
+  </si>
+  <si>
+    <t>INFO:absl:json_outputs='{"model": [{"artifact": {"id": "21227", "type_id": "16", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_4/Trainer/model/22721", "custom_properties": {"name": {"string_value": "model"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "16", "name": "Model"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "Model"}], "model_run": [{"artifact": {"id": "21228", "type_id": "17", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_4/Trainer/model_run/22721", "custom_properties": {"name": {"string_value": "model_run"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "17", "name": "ModelRun"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "ModelRun"}]}'.</t>
+  </si>
+  <si>
+    <t>Focal loss gamma=3.0, alpha=0.75, full dataset from Dylan. Use both keyword embeddings concatenated with synospis output during training of the label tags, but at inference time, appending the keyword embeddings to the output vector (combining approaches from both). The reason we do this is that the precision-recall curve with keywords concat with synopsis is much better than that of synopsis only. Therefore, this approach would have the benefit of both having better tag label vectors, as well as taking the improvement brought by appending the embedding vectors</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.0323
+Precision@5 : 0.025640000000002557
+Precision@10 : 0.021410000000002115
+Recall@1 : 0.00654133333333314
+Recall@5 : 0.026047333333335806
+Recall@10 : 0.04349166666667036
+Accuracy@1 : 0.0323
+Accuracy@5 : 0.11664
+Accuracy@10 : 0.18322
+Coverage@1 : 0.6244131455399061
+Coverage@5 : 0.8826291079812206
+Coverage@10 : 0.95439302481556</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210430155042</t>
+  </si>
+  <si>
+    <t>INFO:absl:json_outputs='{"model": [{"artifact": {"id": "21268", "type_id": "16", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_4/Trainer/model/22754", "custom_properties": {"producer_component": {"string_value": "Trainer"}, "name": {"string_value": "model"}}}, "artifact_type": {"id": "16", "name": "Model"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "Model"}], "model_run": [{"artifact": {"id": "21269", "type_id": "17", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_4/Trainer/model_run/22754", "custom_properties": {"name": {"string_value": "model_run"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "17", "name": "ModelRun"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "ModelRun"}]}'.</t>
+  </si>
+  <si>
+    <t>New bench mark for raw tags and subgenre</t>
+  </si>
+  <si>
+    <t>Do another experiment here: With Dylan's data, without tokens, limit 20 to train, eval on the full set. See how well it performs against exp row 8, and row 16</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.03236
+Precision@5 : 0.0252920000000025
+Precision@10 : 0.02097800000000238
+Recall@1 : 0.006556666666666472
+Recall@5 : 0.025677000000002413
+Recall@10 : 0.04259566666667087
+Accuracy@1 : 0.03236
+Accuracy@5 : 0.115
+Accuracy@10 : 0.17962
+Coverage@1 : 0.6230717639168344
+Coverage@5 : 0.8799463447350772
+Coverage@10 : 0.9517102615694165</t>
+  </si>
+  <si>
+    <t>Focal loss gamma=3.0, alpha=0.85, full dataset from Dylan. Other settings same as above</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_4_20210430214839</t>
+  </si>
+  <si>
+    <t>Results are worse with greater alpha</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Precision@1 0.03318331833183318
+Precision@5 0.024486448644866897
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Precision@10 0.022326232623263977</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Recall@1 0.006636663666366431
+Recall@5 0.024486448644866897
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Recall@10 0.04465246524652795</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Accuracy@1 0.03318331833183318
+Accuracy@5 0.11329132913291329
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Accuracy@10 0.1930793079307931</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Coverage@1 0.6364247311827957
+Coverage@5 0.8494623655913979
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Coverage@10 0.9422043010752689</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -730,6 +883,11 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -758,7 +916,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -782,6 +940,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1099,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1112,7 +1273,8 @@
     <col min="3" max="3" width="51.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="39.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="3"/>
+    <col min="6" max="6" width="45.33203125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1132,102 +1294,102 @@
         <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:6" customFormat="1" ht="204" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="4"/>
       <c r="D2" s="2"/>
       <c r="E2" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" customFormat="1" ht="204" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" customFormat="1" ht="204" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1235,63 +1397,60 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="204" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="204" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1299,33 +1458,30 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="204" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1333,13 +1489,16 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>108</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1347,19 +1506,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>72</v>
+        <v>44</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1367,16 +1520,19 @@
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>56</v>
+      <c r="E19" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1384,19 +1540,16 @@
         <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>73</v>
+        <v>56</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1404,13 +1557,19 @@
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>61</v>
+      <c r="F21" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1418,13 +1577,13 @@
         <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1432,13 +1591,13 @@
         <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1446,13 +1605,13 @@
         <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1460,13 +1619,13 @@
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1474,13 +1633,13 @@
         <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1488,13 +1647,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>86</v>
+        <v>76</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1502,13 +1661,13 @@
         <v>14</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1516,13 +1675,13 @@
         <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1530,13 +1689,13 @@
         <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1544,102 +1703,164 @@
         <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="388" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" s="8" t="s">
+      <c r="F32" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="388" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E33" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="388" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="C41" s="9" t="s">
-        <v>58</v>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="C42" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" location="/pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/a77848d3-ecce-4c1e-980b-e81464cf3922" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/a77848d3-ecce-4c1e-980b-e81464cf3922" xr:uid="{6CADB887-E914-A548-BD60-14E3B72B0825}"/>
-    <hyperlink ref="B6" r:id="rId2" location="/pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/8749b116-3366-4768-bbc9-84655219119b" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/8749b116-3366-4768-bbc9-84655219119b" xr:uid="{4D8C4DBB-6579-EA45-8B22-D2EF85202988}"/>
-    <hyperlink ref="B4" r:id="rId3" location="/pipelines/details/2d03a5e5-98f6-4227-8359-7df4434bba59/version/fa6e652e-b9b0-40dc-a4ad-9d5fc0847b36" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/2d03a5e5-98f6-4227-8359-7df4434bba59/version/fa6e652e-b9b0-40dc-a4ad-9d5fc0847b36" xr:uid="{039C9CF1-62DD-4F4B-883C-5A30A0D21833}"/>
-    <hyperlink ref="B7" r:id="rId4" location="/pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/b83837ad-21ec-4b02-883a-adde0a4ac481" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/b83837ad-21ec-4b02-883a-adde0a4ac481" xr:uid="{4B99E3D9-13DC-3844-9693-8F849FAAE0C1}"/>
-    <hyperlink ref="B8" r:id="rId5" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/886039c0-854f-41eb-93a2-bb207ca38627" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/886039c0-854f-41eb-93a2-bb207ca38627" xr:uid="{BE451817-B1C2-484D-9159-FBE548FAAB28}"/>
-    <hyperlink ref="B9" r:id="rId6" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0f8ad371-21aa-4938-bf60-984f0b06c079" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0f8ad371-21aa-4938-bf60-984f0b06c079" xr:uid="{2ACC4C89-1A2A-304C-A9E1-7F526EC13E5F}"/>
-    <hyperlink ref="B10" r:id="rId7" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/4f1ad934-d906-44e7-9fe2-7bf0c1817de1" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/4f1ad934-d906-44e7-9fe2-7bf0c1817de1" xr:uid="{F48B702F-8538-2145-A364-4423DF860EAC}"/>
-    <hyperlink ref="B11" r:id="rId8" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5106c84f-991f-4146-867e-cc3d76eb0813" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5106c84f-991f-4146-867e-cc3d76eb0813" xr:uid="{5513A0CA-55BE-3E48-BEC4-C38D78FC1216}"/>
-    <hyperlink ref="B12" r:id="rId9" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/18e914b3-fabc-43ed-bf9b-53004e624a6f" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/18e914b3-fabc-43ed-bf9b-53004e624a6f" xr:uid="{58D3158F-006A-F146-B3B5-8741FD236400}"/>
-    <hyperlink ref="B14" r:id="rId10" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/f013bd7f-c122-4130-9817-733ed0251dd5" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/f013bd7f-c122-4130-9817-733ed0251dd5" xr:uid="{8D46A18F-6877-FD49-9F74-C1A476B1E63E}"/>
-    <hyperlink ref="B13" r:id="rId11" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9ae49c61-0512-4ae3-ab82-aaf630837157" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9ae49c61-0512-4ae3-ab82-aaf630837157" xr:uid="{BAA3A710-C9BA-944B-A594-F9E4859C8A28}"/>
-    <hyperlink ref="B15" r:id="rId12" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/8d0e5341-e919-4d22-bb9d-5a235f635c29" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/8d0e5341-e919-4d22-bb9d-5a235f635c29" xr:uid="{C852A73B-8BFA-FB4C-8C90-A66826250654}"/>
-    <hyperlink ref="B18" r:id="rId13" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/49bfd0d1-a4bc-4d7c-87f3-2a5fc4b7201f" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/49bfd0d1-a4bc-4d7c-87f3-2a5fc4b7201f" xr:uid="{B2E8A652-23BB-154F-9D87-8BC59975C310}"/>
-    <hyperlink ref="A18" r:id="rId14" location="/runs/details/7b817ba5-5839-478c-b1ff-b6246bae21f0" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/7b817ba5-5839-478c-b1ff-b6246bae21f0" xr:uid="{CFB6E5C7-5864-B648-8500-CF112866B8CE}"/>
-    <hyperlink ref="A14" r:id="rId15" location="/runs/details/f1163bd7-b8d4-445a-a42e-4edaf56e8d9f" xr:uid="{68E663FB-0D8C-984C-8C2A-917B4ADB3494}"/>
-    <hyperlink ref="A15" r:id="rId16" location="/runs/details/05d53fcc-72d4-4236-bdde-621a2fb04b0c" xr:uid="{18290361-86B5-0F44-8E73-897BF3FBD285}"/>
-    <hyperlink ref="A16" r:id="rId17" location="/runs/details/db2a5779-c6c8-4b52-8552-d9a96441b5cd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/db2a5779-c6c8-4b52-8552-d9a96441b5cd" xr:uid="{BCFF0B7D-D07A-3949-A741-2303C5EB6FD5}"/>
-    <hyperlink ref="B16" r:id="rId18" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/beb3555c-3ca6-4dcb-a3ce-ce5d17db9deb" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/beb3555c-3ca6-4dcb-a3ce-ce5d17db9deb" xr:uid="{138789EA-3C7F-F043-8D4E-25DFD8597CA3}"/>
-    <hyperlink ref="A17" r:id="rId19" location="/runs/details/7dc1fe4b-4048-40b5-aa4c-a2109ccc5446" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/7dc1fe4b-4048-40b5-aa4c-a2109ccc5446" xr:uid="{82CC4711-3C00-0A47-B528-F4D0AE38528A}"/>
-    <hyperlink ref="B17" r:id="rId20" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5430845c-abf4-4986-950f-a7475c36debd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5430845c-abf4-4986-950f-a7475c36debd" xr:uid="{D822687D-B057-2649-9288-155ACA16B32F}"/>
-    <hyperlink ref="B19" r:id="rId21" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/491ce751-af86-4aa2-b8e6-b8a5c182593a" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/491ce751-af86-4aa2-b8e6-b8a5c182593a" xr:uid="{57618230-5285-324A-A1A4-3B3F11257C75}"/>
-    <hyperlink ref="A19" r:id="rId22" location="/runs/details/66f64249-e696-4c9d-94ad-55d4d6cca0bd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/66f64249-e696-4c9d-94ad-55d4d6cca0bd" xr:uid="{049A3D84-8C37-9A41-A40A-FDE3B5FEA125}"/>
-    <hyperlink ref="B20" r:id="rId23" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/db283ecc-ea66-480c-9b97-67dfb2d18268" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/db283ecc-ea66-480c-9b97-67dfb2d18268" xr:uid="{531383F3-0E15-D845-8D1F-1B46D231F1B8}"/>
-    <hyperlink ref="A20" r:id="rId24" location="/runs/details/cb96d58a-767d-46f6-9976-d388c84d2452" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/cb96d58a-767d-46f6-9976-d388c84d2452" xr:uid="{35D78386-8FD6-BF44-9D21-F604191E59F6}"/>
-    <hyperlink ref="A21" r:id="rId25" location="/runs/details/c2e23f01-d8f6-4dfd-8641-69b71d6ca5c0" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/c2e23f01-d8f6-4dfd-8641-69b71d6ca5c0" xr:uid="{5A0CA5BD-2369-094C-A946-CC441D5C53D2}"/>
-    <hyperlink ref="B21" r:id="rId26" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/a817efde-157a-4684-ac7c-99655a17bf41" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/a817efde-157a-4684-ac7c-99655a17bf41" xr:uid="{5B4EAE82-DDB6-414C-9031-37D8F76824C9}"/>
-    <hyperlink ref="A22" r:id="rId27" location="/runs/details/200dcbf7-eeb4-4e08-919c-cc17ad252095" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/200dcbf7-eeb4-4e08-919c-cc17ad252095" xr:uid="{2C4F631C-D961-0643-B6FE-CA44414997DB}"/>
-    <hyperlink ref="B22" r:id="rId28" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/8b33536d-b697-4c9e-8378-e7f95236d3ee" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/8b33536d-b697-4c9e-8378-e7f95236d3ee" xr:uid="{DDFCA432-3B61-D541-ABFD-04D754A6F6D7}"/>
-    <hyperlink ref="B23" r:id="rId29" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/1ea8e64b-cf0c-4ac8-ab5f-0c720739b74e" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/1ea8e64b-cf0c-4ac8-ab5f-0c720739b74e" xr:uid="{3FADE671-7909-2944-923E-127903BE8B4C}"/>
-    <hyperlink ref="A23" r:id="rId30" location="/runs/details/f5869dfd-508d-4e09-9492-fa4c0ec4c3b3" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/f5869dfd-508d-4e09-9492-fa4c0ec4c3b3" xr:uid="{5B6141B6-E10B-E149-88D6-AA0DCD5FFC33}"/>
-    <hyperlink ref="A24" r:id="rId31" location="/runs/details/4ffd7518-610e-4076-9d8e-83f05da77f4d" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/4ffd7518-610e-4076-9d8e-83f05da77f4d" xr:uid="{3BC3E3A8-D78F-994E-8FA8-8F224FD66352}"/>
-    <hyperlink ref="A25" r:id="rId32" location="/runs/details/565a7705-d985-440f-87bd-171f80a513f4" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/565a7705-d985-440f-87bd-171f80a513f4" xr:uid="{2CBF6DF0-D432-F943-B5FB-1A34A7E37FF9}"/>
-    <hyperlink ref="A26" r:id="rId33" location="/runs/details/7bd299b1-442e-43a4-9ddb-b868d3cc2e84" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/7bd299b1-442e-43a4-9ddb-b868d3cc2e84" xr:uid="{79C1D270-3767-D24D-B35C-9C607FDB8237}"/>
-    <hyperlink ref="B26" r:id="rId34" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/b10ae4e6-a067-4240-8de4-e09e7fab1fab" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/b10ae4e6-a067-4240-8de4-e09e7fab1fab" xr:uid="{1E249273-8AA9-CA4D-84D5-E3B124DE49E1}"/>
-    <hyperlink ref="B27" r:id="rId35" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0ad5f912-448f-46a7-baac-23380e3ebde1" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0ad5f912-448f-46a7-baac-23380e3ebde1" xr:uid="{68186EC4-3B21-6341-B7EC-6846DDB5F303}"/>
-    <hyperlink ref="A27" r:id="rId36" location="/runs/details/fe703800-5ed4-48a7-8959-ca9cd00669a6" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/fe703800-5ed4-48a7-8959-ca9cd00669a6" xr:uid="{7C97D0F8-ECA2-744D-8D9C-81D113EA2772}"/>
-    <hyperlink ref="A28" r:id="rId37" location="/runs/details/85ef22c4-3bfb-4c8a-abb0-6f5a7ef4bd3c" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/85ef22c4-3bfb-4c8a-abb0-6f5a7ef4bd3c" xr:uid="{74EF2AAC-46D5-8D47-BD77-DA5116E08B0D}"/>
-    <hyperlink ref="B28" r:id="rId38" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9604be9a-0bc3-4f4b-b3fe-573c43c58614" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9604be9a-0bc3-4f4b-b3fe-573c43c58614" xr:uid="{00E298FB-22B7-5A45-8815-706BFE7141AD}"/>
-    <hyperlink ref="A29" r:id="rId39" location="/runs/details/2173aac9-2fc6-41fa-be94-a81a105abe56" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/2173aac9-2fc6-41fa-be94-a81a105abe56" xr:uid="{F172878E-4B3A-2540-9138-C75A12D2E948}"/>
-    <hyperlink ref="B29" r:id="rId40" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/46949b0f-4756-4035-8bc3-18e961d85545" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/46949b0f-4756-4035-8bc3-18e961d85545" xr:uid="{33762F08-B4E2-EA40-AF59-D34CA2C37B89}"/>
-    <hyperlink ref="B30" r:id="rId41" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/618cb506-ab3b-40fd-b13a-c432466f5a55" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/618cb506-ab3b-40fd-b13a-c432466f5a55" xr:uid="{35066E55-C490-444F-90CF-EC8B6943ED77}"/>
-    <hyperlink ref="A30" r:id="rId42" location="/runs/details/0ece7dde-344b-4e1e-a84c-48075de44051" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/0ece7dde-344b-4e1e-a84c-48075de44051" xr:uid="{3828495F-E236-8448-A21D-54ADF5F1F67C}"/>
-    <hyperlink ref="A31" r:id="rId43" location="/runs/details/9908e4bf-71ab-4f5b-8c7f-c4b374bf7a65" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/9908e4bf-71ab-4f5b-8c7f-c4b374bf7a65" xr:uid="{AED4D5B8-7808-3241-A1C4-108A980111D2}"/>
-    <hyperlink ref="B31" r:id="rId44" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/7cea8693-b60a-4622-a597-3d370feda18d" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/7cea8693-b60a-4622-a597-3d370feda18d" xr:uid="{A6960C78-B1EF-8B45-97D1-9076EC413127}"/>
+    <hyperlink ref="B6" r:id="rId1" location="/pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/a77848d3-ecce-4c1e-980b-e81464cf3922" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/a77848d3-ecce-4c1e-980b-e81464cf3922" xr:uid="{6CADB887-E914-A548-BD60-14E3B72B0825}"/>
+    <hyperlink ref="B7" r:id="rId2" location="/pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/8749b116-3366-4768-bbc9-84655219119b" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/8749b116-3366-4768-bbc9-84655219119b" xr:uid="{4D8C4DBB-6579-EA45-8B22-D2EF85202988}"/>
+    <hyperlink ref="B5" r:id="rId3" location="/pipelines/details/2d03a5e5-98f6-4227-8359-7df4434bba59/version/fa6e652e-b9b0-40dc-a4ad-9d5fc0847b36" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/2d03a5e5-98f6-4227-8359-7df4434bba59/version/fa6e652e-b9b0-40dc-a4ad-9d5fc0847b36" xr:uid="{039C9CF1-62DD-4F4B-883C-5A30A0D21833}"/>
+    <hyperlink ref="B8" r:id="rId4" location="/pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/b83837ad-21ec-4b02-883a-adde0a4ac481" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/5f53f2c4-1ce2-4a3d-88a9-368faee98556/version/b83837ad-21ec-4b02-883a-adde0a4ac481" xr:uid="{4B99E3D9-13DC-3844-9693-8F849FAAE0C1}"/>
+    <hyperlink ref="B9" r:id="rId5" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/886039c0-854f-41eb-93a2-bb207ca38627" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/886039c0-854f-41eb-93a2-bb207ca38627" xr:uid="{BE451817-B1C2-484D-9159-FBE548FAAB28}"/>
+    <hyperlink ref="B10" r:id="rId6" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0f8ad371-21aa-4938-bf60-984f0b06c079" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0f8ad371-21aa-4938-bf60-984f0b06c079" xr:uid="{2ACC4C89-1A2A-304C-A9E1-7F526EC13E5F}"/>
+    <hyperlink ref="B11" r:id="rId7" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/4f1ad934-d906-44e7-9fe2-7bf0c1817de1" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/4f1ad934-d906-44e7-9fe2-7bf0c1817de1" xr:uid="{F48B702F-8538-2145-A364-4423DF860EAC}"/>
+    <hyperlink ref="B12" r:id="rId8" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5106c84f-991f-4146-867e-cc3d76eb0813" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5106c84f-991f-4146-867e-cc3d76eb0813" xr:uid="{5513A0CA-55BE-3E48-BEC4-C38D78FC1216}"/>
+    <hyperlink ref="B13" r:id="rId9" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/18e914b3-fabc-43ed-bf9b-53004e624a6f" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/18e914b3-fabc-43ed-bf9b-53004e624a6f" xr:uid="{58D3158F-006A-F146-B3B5-8741FD236400}"/>
+    <hyperlink ref="B15" r:id="rId10" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/f013bd7f-c122-4130-9817-733ed0251dd5" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/f013bd7f-c122-4130-9817-733ed0251dd5" xr:uid="{8D46A18F-6877-FD49-9F74-C1A476B1E63E}"/>
+    <hyperlink ref="B14" r:id="rId11" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9ae49c61-0512-4ae3-ab82-aaf630837157" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9ae49c61-0512-4ae3-ab82-aaf630837157" xr:uid="{BAA3A710-C9BA-944B-A594-F9E4859C8A28}"/>
+    <hyperlink ref="B16" r:id="rId12" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/8d0e5341-e919-4d22-bb9d-5a235f635c29" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/8d0e5341-e919-4d22-bb9d-5a235f635c29" xr:uid="{C852A73B-8BFA-FB4C-8C90-A66826250654}"/>
+    <hyperlink ref="B19" r:id="rId13" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/49bfd0d1-a4bc-4d7c-87f3-2a5fc4b7201f" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/49bfd0d1-a4bc-4d7c-87f3-2a5fc4b7201f" xr:uid="{B2E8A652-23BB-154F-9D87-8BC59975C310}"/>
+    <hyperlink ref="A19" r:id="rId14" location="/runs/details/7b817ba5-5839-478c-b1ff-b6246bae21f0" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/7b817ba5-5839-478c-b1ff-b6246bae21f0" xr:uid="{CFB6E5C7-5864-B648-8500-CF112866B8CE}"/>
+    <hyperlink ref="A15" r:id="rId15" location="/runs/details/f1163bd7-b8d4-445a-a42e-4edaf56e8d9f" xr:uid="{68E663FB-0D8C-984C-8C2A-917B4ADB3494}"/>
+    <hyperlink ref="A16" r:id="rId16" location="/runs/details/05d53fcc-72d4-4236-bdde-621a2fb04b0c" xr:uid="{18290361-86B5-0F44-8E73-897BF3FBD285}"/>
+    <hyperlink ref="A17" r:id="rId17" location="/runs/details/db2a5779-c6c8-4b52-8552-d9a96441b5cd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/db2a5779-c6c8-4b52-8552-d9a96441b5cd" xr:uid="{BCFF0B7D-D07A-3949-A741-2303C5EB6FD5}"/>
+    <hyperlink ref="B17" r:id="rId18" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/beb3555c-3ca6-4dcb-a3ce-ce5d17db9deb" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/beb3555c-3ca6-4dcb-a3ce-ce5d17db9deb" xr:uid="{138789EA-3C7F-F043-8D4E-25DFD8597CA3}"/>
+    <hyperlink ref="A18" r:id="rId19" location="/runs/details/7dc1fe4b-4048-40b5-aa4c-a2109ccc5446" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/7dc1fe4b-4048-40b5-aa4c-a2109ccc5446" xr:uid="{82CC4711-3C00-0A47-B528-F4D0AE38528A}"/>
+    <hyperlink ref="B18" r:id="rId20" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5430845c-abf4-4986-950f-a7475c36debd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/5430845c-abf4-4986-950f-a7475c36debd" xr:uid="{D822687D-B057-2649-9288-155ACA16B32F}"/>
+    <hyperlink ref="B20" r:id="rId21" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/491ce751-af86-4aa2-b8e6-b8a5c182593a" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/491ce751-af86-4aa2-b8e6-b8a5c182593a" xr:uid="{57618230-5285-324A-A1A4-3B3F11257C75}"/>
+    <hyperlink ref="A20" r:id="rId22" location="/runs/details/66f64249-e696-4c9d-94ad-55d4d6cca0bd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/66f64249-e696-4c9d-94ad-55d4d6cca0bd" xr:uid="{049A3D84-8C37-9A41-A40A-FDE3B5FEA125}"/>
+    <hyperlink ref="B21" r:id="rId23" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/db283ecc-ea66-480c-9b97-67dfb2d18268" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/db283ecc-ea66-480c-9b97-67dfb2d18268" xr:uid="{531383F3-0E15-D845-8D1F-1B46D231F1B8}"/>
+    <hyperlink ref="A21" r:id="rId24" location="/runs/details/cb96d58a-767d-46f6-9976-d388c84d2452" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/cb96d58a-767d-46f6-9976-d388c84d2452" xr:uid="{35D78386-8FD6-BF44-9D21-F604191E59F6}"/>
+    <hyperlink ref="A22" r:id="rId25" location="/runs/details/c2e23f01-d8f6-4dfd-8641-69b71d6ca5c0" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/c2e23f01-d8f6-4dfd-8641-69b71d6ca5c0" xr:uid="{5A0CA5BD-2369-094C-A946-CC441D5C53D2}"/>
+    <hyperlink ref="B22" r:id="rId26" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/a817efde-157a-4684-ac7c-99655a17bf41" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/a817efde-157a-4684-ac7c-99655a17bf41" xr:uid="{5B4EAE82-DDB6-414C-9031-37D8F76824C9}"/>
+    <hyperlink ref="A23" r:id="rId27" location="/runs/details/200dcbf7-eeb4-4e08-919c-cc17ad252095" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/200dcbf7-eeb4-4e08-919c-cc17ad252095" xr:uid="{2C4F631C-D961-0643-B6FE-CA44414997DB}"/>
+    <hyperlink ref="B23" r:id="rId28" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/8b33536d-b697-4c9e-8378-e7f95236d3ee" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/8b33536d-b697-4c9e-8378-e7f95236d3ee" xr:uid="{DDFCA432-3B61-D541-ABFD-04D754A6F6D7}"/>
+    <hyperlink ref="B24" r:id="rId29" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/1ea8e64b-cf0c-4ac8-ab5f-0c720739b74e" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/1ea8e64b-cf0c-4ac8-ab5f-0c720739b74e" xr:uid="{3FADE671-7909-2944-923E-127903BE8B4C}"/>
+    <hyperlink ref="A24" r:id="rId30" location="/runs/details/f5869dfd-508d-4e09-9492-fa4c0ec4c3b3" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/f5869dfd-508d-4e09-9492-fa4c0ec4c3b3" xr:uid="{5B6141B6-E10B-E149-88D6-AA0DCD5FFC33}"/>
+    <hyperlink ref="A25" r:id="rId31" location="/runs/details/4ffd7518-610e-4076-9d8e-83f05da77f4d" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/4ffd7518-610e-4076-9d8e-83f05da77f4d" xr:uid="{3BC3E3A8-D78F-994E-8FA8-8F224FD66352}"/>
+    <hyperlink ref="A26" r:id="rId32" location="/runs/details/565a7705-d985-440f-87bd-171f80a513f4" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/565a7705-d985-440f-87bd-171f80a513f4" xr:uid="{2CBF6DF0-D432-F943-B5FB-1A34A7E37FF9}"/>
+    <hyperlink ref="A27" r:id="rId33" location="/runs/details/7bd299b1-442e-43a4-9ddb-b868d3cc2e84" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/7bd299b1-442e-43a4-9ddb-b868d3cc2e84" xr:uid="{79C1D270-3767-D24D-B35C-9C607FDB8237}"/>
+    <hyperlink ref="B27" r:id="rId34" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/b10ae4e6-a067-4240-8de4-e09e7fab1fab" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/b10ae4e6-a067-4240-8de4-e09e7fab1fab" xr:uid="{1E249273-8AA9-CA4D-84D5-E3B124DE49E1}"/>
+    <hyperlink ref="B28" r:id="rId35" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0ad5f912-448f-46a7-baac-23380e3ebde1" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/0ad5f912-448f-46a7-baac-23380e3ebde1" xr:uid="{68186EC4-3B21-6341-B7EC-6846DDB5F303}"/>
+    <hyperlink ref="A28" r:id="rId36" location="/runs/details/fe703800-5ed4-48a7-8959-ca9cd00669a6" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/fe703800-5ed4-48a7-8959-ca9cd00669a6" xr:uid="{7C97D0F8-ECA2-744D-8D9C-81D113EA2772}"/>
+    <hyperlink ref="A29" r:id="rId37" location="/runs/details/85ef22c4-3bfb-4c8a-abb0-6f5a7ef4bd3c" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/85ef22c4-3bfb-4c8a-abb0-6f5a7ef4bd3c" xr:uid="{74EF2AAC-46D5-8D47-BD77-DA5116E08B0D}"/>
+    <hyperlink ref="B29" r:id="rId38" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9604be9a-0bc3-4f4b-b3fe-573c43c58614" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9604be9a-0bc3-4f4b-b3fe-573c43c58614" xr:uid="{00E298FB-22B7-5A45-8815-706BFE7141AD}"/>
+    <hyperlink ref="A30" r:id="rId39" location="/runs/details/2173aac9-2fc6-41fa-be94-a81a105abe56" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/2173aac9-2fc6-41fa-be94-a81a105abe56" xr:uid="{F172878E-4B3A-2540-9138-C75A12D2E948}"/>
+    <hyperlink ref="B30" r:id="rId40" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/46949b0f-4756-4035-8bc3-18e961d85545" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/46949b0f-4756-4035-8bc3-18e961d85545" xr:uid="{33762F08-B4E2-EA40-AF59-D34CA2C37B89}"/>
+    <hyperlink ref="B31" r:id="rId41" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/618cb506-ab3b-40fd-b13a-c432466f5a55" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/618cb506-ab3b-40fd-b13a-c432466f5a55" xr:uid="{35066E55-C490-444F-90CF-EC8B6943ED77}"/>
+    <hyperlink ref="A31" r:id="rId42" location="/runs/details/0ece7dde-344b-4e1e-a84c-48075de44051" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/0ece7dde-344b-4e1e-a84c-48075de44051" xr:uid="{3828495F-E236-8448-A21D-54ADF5F1F67C}"/>
+    <hyperlink ref="A32" r:id="rId43" location="/runs/details/9908e4bf-71ab-4f5b-8c7f-c4b374bf7a65" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/9908e4bf-71ab-4f5b-8c7f-c4b374bf7a65" xr:uid="{AED4D5B8-7808-3241-A1C4-108A980111D2}"/>
+    <hyperlink ref="B32" r:id="rId44" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/7cea8693-b60a-4622-a597-3d370feda18d" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/7cea8693-b60a-4622-a597-3d370feda18d" xr:uid="{A6960C78-B1EF-8B45-97D1-9076EC413127}"/>
+    <hyperlink ref="A33" r:id="rId45" location="/runs/details/70d89993-96a9-4b17-b42a-6cc16b18b7af" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/70d89993-96a9-4b17-b42a-6cc16b18b7af" xr:uid="{38CFF0C2-FE2E-B74F-BAC8-F334EECE624A}"/>
+    <hyperlink ref="B33" r:id="rId46" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/fb9231f1-5906-46a2-a094-8fd0f0a0ec25" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/fb9231f1-5906-46a2-a094-8fd0f0a0ec25" xr:uid="{70F18E10-9D0E-264A-9EE1-C7930C2567F3}"/>
+    <hyperlink ref="A34" r:id="rId47" location="/runs/details/63d5d993-1628-4f90-8078-463d62c63ac3" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/63d5d993-1628-4f90-8078-463d62c63ac3" xr:uid="{0B3188D3-CC6E-5644-B1F0-C5E38515BA39}"/>
+    <hyperlink ref="B34" r:id="rId48" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9a4e46c6-3af6-466b-8f6c-50158b51164a" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9a4e46c6-3af6-466b-8f6c-50158b51164a" xr:uid="{09F5DEDE-9DC1-3F4B-8974-D7905C03E239}"/>
+    <hyperlink ref="B35" r:id="rId49" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/b8519c7c-fc95-41ec-abba-6ff77c4a103d" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/b8519c7c-fc95-41ec-abba-6ff77c4a103d" xr:uid="{58B9CF88-F75A-624B-940A-CA1C90B89F81}"/>
+    <hyperlink ref="A35" r:id="rId50" location="/runs/details/07885788-41c1-44a0-ab2a-f2320aad32d9" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/07885788-41c1-44a0-ab2a-f2320aad32d9" xr:uid="{BA5E7F1D-BF72-714B-8C76-1DE6CEEAAAF7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
try append only at predict
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7F18D6-3C4B-BD44-ACAF-E6A921B2ADDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E923459-5AA6-254F-9572-947EF7E7E8B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="116">
   <si>
     <t>Model Version</t>
   </si>
@@ -829,6 +829,12 @@
       </rPr>
       <t>Coverage@10 0.9422043010752689</t>
     </r>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_5</t>
+  </si>
+  <si>
+    <t>Focal loss gamma=3.0, alpha=0.75, full dataset with full tags from Dylan.</t>
   </si>
 </sst>
 </file>
@@ -1262,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1780,9 +1786,16 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
@@ -1861,6 +1874,8 @@
     <hyperlink ref="B34" r:id="rId48" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9a4e46c6-3af6-466b-8f6c-50158b51164a" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/9a4e46c6-3af6-466b-8f6c-50158b51164a" xr:uid="{09F5DEDE-9DC1-3F4B-8974-D7905C03E239}"/>
     <hyperlink ref="B35" r:id="rId49" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/b8519c7c-fc95-41ec-abba-6ff77c4a103d" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/b8519c7c-fc95-41ec-abba-6ff77c4a103d" xr:uid="{58B9CF88-F75A-624B-940A-CA1C90B89F81}"/>
     <hyperlink ref="A35" r:id="rId50" location="/runs/details/07885788-41c1-44a0-ab2a-f2320aad32d9" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/07885788-41c1-44a0-ab2a-f2320aad32d9" xr:uid="{BA5E7F1D-BF72-714B-8C76-1DE6CEEAAAF7}"/>
+    <hyperlink ref="A36" r:id="rId51" location="/runs/details/4f1aa313-cbe0-4e90-b7e8-8f9bd7fe01dd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/4f1aa313-cbe0-4e90-b7e8-8f9bd7fe01dd" xr:uid="{AF761F73-506C-524A-B385-CE616EEEA921}"/>
+    <hyperlink ref="B36" r:id="rId52" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/ce0d5acc-4c98-454a-ad0a-d603424d9973" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/ce0d5acc-4c98-454a-ad0a-d603424d9973" xr:uid="{AE5B90E1-A727-7F4B-BCF8-EB928A5AD98C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
correct eval join problem
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E923459-5AA6-254F-9572-947EF7E7E8B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3F2BBA-C0F1-B440-A9DC-13D717BB7E60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="125">
   <si>
     <t>Model Version</t>
   </si>
@@ -682,20 +682,6 @@
   </si>
   <si>
     <t>metadata_dev_edc_base_0_0_4_20210429224329</t>
-  </si>
-  <si>
-    <t>Precision@1 : 0.03
-Precision@5 : 0.024452000000002354
-Precision@10 : 0.02106600000000236
-Recall@1 : 0.0060576666666665
-Recall@5 : 0.024704666666668935
-Recall@10 : 0.042569333333337775
-Accuracy@1 : 0.03
-Accuracy@5 : 0.1117
-Accuracy@10 : 0.18198
-Coverage@1 : 0.5151311365164761
-Coverage@5 : 0.7881640887693342
-Coverage@10 : 0.8863483523873571</t>
   </si>
   <si>
     <t>INFO:absl:json_outputs='{"model": [{"artifact": {"id": "21227", "type_id": "16", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_4/Trainer/model/22721", "custom_properties": {"name": {"string_value": "model"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "16", "name": "Model"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "Model"}], "model_run": [{"artifact": {"id": "21228", "type_id": "17", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_4/Trainer/model_run/22721", "custom_properties": {"name": {"string_value": "model_run"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "17", "name": "ModelRun"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "ModelRun"}]}'.</t>
@@ -834,14 +820,88 @@
     <t>metadata_dev_edc_base_0_0_5</t>
   </si>
   <si>
-    <t>Focal loss gamma=3.0, alpha=0.75, full dataset with full tags from Dylan.</t>
+    <t>Precision@1 : 0.02936
+Precision@5 : 0.025176000000002433
+Precision@10 : 0.021606000000001985
+Recall@1 : 0.005942666666666506
+Recall@5 : 0.025489000000002357
+Recall@10 : 0.04381433333333686
+Accuracy@1 : 0.02936
+Accuracy@5 : 0.11408
+Accuracy@10 : 0.1832
+Coverage@1 : 0.6320375335120644
+Coverage@5 : 0.8833780160857909
+Coverage@10 : 0.9463806970509383</t>
+  </si>
+  <si>
+    <t>Not any better. Slightly better in terms of recall and precision</t>
+  </si>
+  <si>
+    <t>Focal loss gamma=3.0, alpha=0.75, full dataset with full tags from Dylan, feeding keyword embedding before dense, but also append the embeddings afterwards</t>
+  </si>
+  <si>
+    <t>Focal loss gamma=3.0, alpha=0.75, full dataset with full tags from Dylan, feeding keyword embedding before dense only</t>
+  </si>
+  <si>
+    <t>If the goal is to trying to make inference on the data of ContentMetadataView (CMV), why not just train on these data only? Specifically, just extract synopsis, keywords (TitleTags+TitleType), and labels as TitleGenres, etc. Focal loss gamma=3.0, alpha=0.75, full dataset from Dylan, with full label tags</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_5_20210503200936</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.0302
+Precision@5 : 0.025436000000002578
+Precision@10 : 0.02156200000000206
+Recall@1 : 0.006087999999999829
+Recall@5 : 0.02566733333333583
+Recall@10 : 0.043599000000003815
+Accuracy@1 : 0.0302
+Accuracy@5 : 0.11576
+Accuracy@10 : 0.1851
+Coverage@1 : 0.3894101876675603
+Coverage@5 : 0.6407506702412868
+Coverage@10 : 0.7540214477211796</t>
+  </si>
+  <si>
+    <t>INFO:absl:json_outputs='{"model": [{"artifact": {"id": "21923", "type_id": "16", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_5/Trainer/model/23222", "custom_properties": {"name": {"string_value": "model"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "16", "name": "Model"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "Model"}], "model_run": [{"artifact": {"id": "21924", "type_id": "17", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_5/Trainer/model_run/23222", "custom_properties": {"name": {"string_value": "model_run"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "17", "name": "ModelRun"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "ModelRun"}]}'.</t>
+  </si>
+  <si>
+    <t>No need to get this additional data involved</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.04634
+Precision@5 : 0.031516000000003305
+Precision@10 : 0.025086000000000518
+Recall@1 : 0.009267999999999645
+Recall@5 : 0.03153200000000331
+Recall@10 : 0.050188000000001044
+Accuracy@1 : 0.04634
+Accuracy@5 : 0.13138
+Accuracy@10 : 0.19806
+Coverage@1 : 0.49831973115698514
+Coverage@5 : 0.7676428228516563
+Coverage@10 : 0.8785405664906385</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.03876
+Precision@5 : 0.028208000000003
+Precision@10 : 0.02415600000000068
+Recall@1 : 0.007751999999999731
+Recall@5 : 0.02822400000000301
+Recall@10 : 0.04832800000000136
+Accuracy@1 : 0.03876
+Accuracy@5 : 0.12316
+Accuracy@10 : 0.1936
+Coverage@1 : 0.39222275564090253
+Coverage@5 : 0.6164186269803168
+Coverage@10 : 0.7364378300528085</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -894,6 +954,11 @@
       <color theme="5"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -922,7 +987,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -949,6 +1014,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1266,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1327,13 +1395,13 @@
     </row>
     <row r="4" spans="1:6" customFormat="1" ht="204" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="6"/>
       <c r="E4" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1498,7 +1566,7 @@
         <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>43</v>
@@ -1746,10 +1814,10 @@
         <v>98</v>
       </c>
       <c r="E33" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="388" x14ac:dyDescent="0.2">
@@ -1757,16 +1825,16 @@
         <v>14</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1774,51 +1842,97 @@
         <v>14</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="E35" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+    </row>
+    <row r="37" spans="1:6" ht="388" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
+      <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
+      <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="C42" s="9" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="C45" s="9" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1875,7 +1989,11 @@
     <hyperlink ref="B35" r:id="rId49" location="/pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/b8519c7c-fc95-41ec-abba-6ff77c4a103d" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/6ba19308-c6b1-4af5-933d-4a26af0c1130/version/b8519c7c-fc95-41ec-abba-6ff77c4a103d" xr:uid="{58B9CF88-F75A-624B-940A-CA1C90B89F81}"/>
     <hyperlink ref="A35" r:id="rId50" location="/runs/details/07885788-41c1-44a0-ab2a-f2320aad32d9" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/07885788-41c1-44a0-ab2a-f2320aad32d9" xr:uid="{BA5E7F1D-BF72-714B-8C76-1DE6CEEAAAF7}"/>
     <hyperlink ref="A36" r:id="rId51" location="/runs/details/4f1aa313-cbe0-4e90-b7e8-8f9bd7fe01dd" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/4f1aa313-cbe0-4e90-b7e8-8f9bd7fe01dd" xr:uid="{AF761F73-506C-524A-B385-CE616EEEA921}"/>
-    <hyperlink ref="B36" r:id="rId52" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/ce0d5acc-4c98-454a-ad0a-d603424d9973" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/ce0d5acc-4c98-454a-ad0a-d603424d9973" xr:uid="{AE5B90E1-A727-7F4B-BCF8-EB928A5AD98C}"/>
+    <hyperlink ref="B36" r:id="rId52" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/ce0d5acc-4c98-454a-ad0a-d603424d9973" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/ce0d5acc-4c98-454a-ad0a-d603424d9973" xr:uid="{73220AB8-BBEB-9E42-9D20-4D9C0645EEC0}"/>
+    <hyperlink ref="A38" r:id="rId53" location="/runs/details/1acd71f1-dc2e-4328-8290-9ae660e416f1" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/1acd71f1-dc2e-4328-8290-9ae660e416f1" xr:uid="{7D2FAAE4-3BFA-B44A-81D5-30B86252D767}"/>
+    <hyperlink ref="B38" r:id="rId54" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/d1514788-a6a1-4858-84c4-6114fd8e6605" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/d1514788-a6a1-4858-84c4-6114fd8e6605" xr:uid="{C6174D00-D4D4-A94B-BE46-19AFFEC5F22F}"/>
+    <hyperlink ref="B37" r:id="rId55" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/d1514788-a6a1-4858-84c4-6114fd8e6605" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/d1514788-a6a1-4858-84c4-6114fd8e6605" xr:uid="{EA435A4C-05DA-924B-9D7F-6C335DD96237}"/>
+    <hyperlink ref="A37" r:id="rId56" location="/runs/details/1acd71f1-dc2e-4328-8290-9ae660e416f1" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/1acd71f1-dc2e-4328-8290-9ae660e416f1" xr:uid="{F1166A23-FE14-8949-9B5C-7DA2A0EBCE8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
try full bert with multi lingual
</commit_message>
<xml_diff>
--- a/training/notebooks/Experiment_logs.xlsx
+++ b/training/notebooks/Experiment_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwardcui/Documents/Scripts/nbcu-metadata-enhancement/training/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F477EAB5-45BD-F44B-AF44-98FE328439B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22C6AC2-561F-194C-AAF5-DD72D5E9142E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1520" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{81D60B41-89E0-3847-8719-3EDE43445DF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Synopsis_tag_embeddings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="154">
   <si>
     <t>Model Version</t>
   </si>
@@ -934,7 +934,205 @@
 Coverage@10 : 0.8833413346135381</t>
   </si>
   <si>
-    <t>Synopsis + synopsis extracted tokens appended at the output, Dylan's data with 150 tags, focal loss gamma=3.0, alpha=0.75</t>
+    <t>Synopsis + synopsis extracted tokens appended only at the output, Dylan's data with 150 tags, focal loss gamma=3.0, alpha=0.75</t>
+  </si>
+  <si>
+    <t>Synopsis + synopsis extracted tokens appended at both before dense and at the output, Dylan's data with 150 tags, focal loss gamma=3.0, alpha=0.75</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_5_20210504180822</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.01948
+Precision@5 : 0.016216000000000768
+Precision@10 : 0.015046000000001686
+Recall@1 : 0.00389599999999995
+Recall@5 : 0.016216000000000768
+Recall@10 : 0.030092000000003373
+Accuracy@1 : 0.01948
+Accuracy@5 : 0.07598
+Accuracy@10 : 0.13268
+Coverage@1 : 0.3103614457831325
+Coverage@5 : 0.5146987951807229
+Coverage@10 : 0.6187951807228915</t>
+  </si>
+  <si>
+    <t>INFO:absl:json_outputs='{"model": [{"artifact": {"id": "22175", "type_id": "16", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_5/Trainer/model/23407", "custom_properties": {"producer_component": {"string_value": "Trainer"}, "name": {"string_value": "model"}}}, "artifact_type": {"id": "16", "name": "Model"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "Model"}], "model_run": [{"artifact": {"id": "22176", "type_id": "17", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_5/Trainer/model_run/23407", "custom_properties": {"name": {"string_value": "model_run"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "17", "name": "ModelRun"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "ModelRun"}]}'.</t>
+  </si>
+  <si>
+    <t>INFO:absl:json_outputs='{"model": [{"artifact": {"id": "22190", "type_id": "16", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_5/Trainer/model/23415", "custom_properties": {"producer_component": {"string_value": "Trainer"}, "name": {"string_value": "model"}}}, "artifact_type": {"id": "16", "name": "Model"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "Model"}], "model_run": [{"artifact": {"id": "22191", "type_id": "17", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_5/Trainer/model_run/23415", "custom_properties": {"producer_component": {"string_value": "Trainer"}, "name": {"string_value": "model_run"}}}, "artifact_type": {"id": "17", "name": "ModelRun"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "ModelRun"}]}'.</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.01998
+Precision@5 : 0.01667200000000084
+Precision@10 : 0.015382000000001759
+Recall@1 : 0.003995999999999944
+Recall@5 : 0.01667200000000084
+Recall@10 : 0.030764000000003518
+Accuracy@1 : 0.01998
+Accuracy@5 : 0.07804
+Accuracy@10 : 0.13558
+Coverage@1 : 0.3007228915662651
+Coverage@5 : 0.5142168674698795
+Coverage@10 : 0.6130120481927711</t>
+  </si>
+  <si>
+    <t>Synopsis + synopsis extracted tokens appended at both before dense and at the output, Dylan's data with 150 tags, focal loss gamma=3.0, alpha=0.75, with an additional hidden layer</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_5_20210504192854</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.01692
+Precision@5 : 0.01620000000000075
+Precision@10 : 0.014950000000001655
+Recall@1 : 0.0033839999999999786
+Recall@5 : 0.01620000000000075
+Recall@10 : 0.02990000000000331
+Accuracy@1 : 0.01692
+Accuracy@5 : 0.07536
+Accuracy@10 : 0.13136
+Coverage@1 : 0.3344578313253012
+Coverage@5 : 0.5465060240963855
+Coverage@10 : 0.6433734939759036</t>
+  </si>
+  <si>
+    <t>Synopsis + synopsis token + keywords, feeding before dense layer, then concat afterwards, Dylan's data with 150 tags, focal loss gamma=3.0, alpha=0.75.</t>
+  </si>
+  <si>
+    <t>Precision@1 : 0.03224
+Precision@5 : 0.02569200000000256
+Precision@10 : 0.022116000000001714
+Recall@1 : 0.0064479999999998054
+Recall@5 : 0.02569200000000256
+Recall@10 : 0.04423200000000343
+Accuracy@1 : 0.03224
+Accuracy@5 : 0.11638
+Accuracy@10 : 0.18674
+Coverage@1 : 0.432289156626506
+Coverage@5 : 0.7016867469879519
+Coverage@10 : 0.807710843373494</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_5_20210504202531</t>
+  </si>
+  <si>
+    <t>Not significantly better. Keywords is quite important</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_5_20210505210112</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_5_20210505210257</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_5_20210505210429</t>
+  </si>
+  <si>
+    <t>metadata_dev_edc_base_0_0_5_20210505210605</t>
+  </si>
+  <si>
+    <t>INFO:absl:json_outputs='{"model": [{"artifact": {"id": "22050", "type_id": "16", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_5/Trainer/model/23309", "custom_properties": {"producer_component": {"string_value": "Trainer"}, "name": {"string_value": "model"}}}, "artifact_type": {"id": "16", "name": "Model"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "Model"}], "model_run": [{"artifact": {"id": "22051", "type_id": "17", "uri": "gs://metadata-bucket-base/tfx-metadata-dev-pipeline-output/metadata_dev_edc_base_0_0_5/Trainer/model_run/23309", "custom_properties": {"name": {"string_value": "model_run"}, "producer_component": {"string_value": "Trainer"}}}, "artifact_type": {"id": "17", "name": "ModelRun"}, "__artifact_class_module__": "tfx.types.standard_artifacts", "__artifact_class_name__": "ModelRun"}]}'.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Focal Loss tune:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> gamma=3.0, alpha=0.70, inference with titles embeddings</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Focal Loss tune: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gamma=3.0, alpha=0.80, inference with titles embeddings</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Focal Loss tune: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gamma=2.0, alpha=0.75, inference with titles embeddings</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Focal Loss tune: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gamma=4.0, alpha=0.75, inference with titles embeddings</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Focal loss  tune:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> gamma=3.0, alpha=0.75, inference with titles embeddings, with larger BERT model L-8_H-768_A-12</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1368,10 +1566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84215FDD-47D1-7B45-A23B-12A1E06EB55A}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1936,7 +2134,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="388" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>111</v>
       </c>
@@ -1948,6 +2146,9 @@
       </c>
       <c r="E39" s="9" t="s">
         <v>123</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="204" x14ac:dyDescent="0.2">
@@ -1964,7 +2165,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="388" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>111</v>
       </c>
@@ -1974,21 +2175,109 @@
       <c r="C41" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C45" s="12"/>
+      <c r="E41" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="388" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="C49" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2054,6 +2343,20 @@
     <hyperlink ref="A40" r:id="rId60" location="/runs/details/61893f70-af2f-4033-bdf7-17d8fd1ec046" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/61893f70-af2f-4033-bdf7-17d8fd1ec046" xr:uid="{AF67301B-DC0B-234D-BF27-6DB2CF97E6C5}"/>
     <hyperlink ref="B41" r:id="rId61" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/4b3965fc-83ad-49b2-ba89-033a40ac7b53" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/4b3965fc-83ad-49b2-ba89-033a40ac7b53" xr:uid="{916B4B39-63AC-4C49-A2EB-0D7E3F3A5076}"/>
     <hyperlink ref="A41" r:id="rId62" location="/runs/details/b46adf22-b144-4936-99c9-8b2dc693e900" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/b46adf22-b144-4936-99c9-8b2dc693e900" xr:uid="{1E32E1FD-95F5-764E-8B9F-A1BA3F909A52}"/>
+    <hyperlink ref="B42" r:id="rId63" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/47fc0fbb-b3c4-49e5-a73f-aff0577dc1d6" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/47fc0fbb-b3c4-49e5-a73f-aff0577dc1d6" xr:uid="{2F4453E1-CD74-DF4A-BB55-024628C3472E}"/>
+    <hyperlink ref="A42" r:id="rId64" location="/runs/details/a6271192-5a3d-4ca2-9729-699291762f47" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/a6271192-5a3d-4ca2-9729-699291762f47" xr:uid="{D41190D7-696A-6D45-922A-65A4A59F647A}"/>
+    <hyperlink ref="A43" r:id="rId65" location="/runs/details/29b12407-7a4f-42cd-a3a9-99ca5c6a3815" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/29b12407-7a4f-42cd-a3a9-99ca5c6a3815" xr:uid="{977629FE-068E-E34D-A474-0BD47401E72B}"/>
+    <hyperlink ref="B43" r:id="rId66" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/d3dfb511-650c-47a6-843b-07d9cb93c845" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/d3dfb511-650c-47a6-843b-07d9cb93c845" xr:uid="{10D3E35B-513F-9C4A-B313-D09AF3D468DD}"/>
+    <hyperlink ref="A44" r:id="rId67" location="/runs/details/d28011dd-5c2c-4818-a67a-daeb44127c5b" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/d28011dd-5c2c-4818-a67a-daeb44127c5b" xr:uid="{CDA43416-D64D-E546-8E1A-BC933ED5D03C}"/>
+    <hyperlink ref="B44" r:id="rId68" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/f69a94d8-296c-454a-b777-e6f9c7b7b8dc" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/f69a94d8-296c-454a-b777-e6f9c7b7b8dc" xr:uid="{3DBE953B-9F23-664F-84B9-D7D9017C39D0}"/>
+    <hyperlink ref="A45" r:id="rId69" location="/runs/details/b9522807-13ce-41f1-a971-fd6459d43a57" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/b9522807-13ce-41f1-a971-fd6459d43a57" xr:uid="{CE25F74A-32B6-0046-B016-9BFA336F31BE}"/>
+    <hyperlink ref="B45" r:id="rId70" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/2b47e71d-497b-4b63-80a5-b1e1f9df8683" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/2b47e71d-497b-4b63-80a5-b1e1f9df8683" xr:uid="{00BBC97C-701F-204E-877C-C12AE4083F7C}"/>
+    <hyperlink ref="A46" r:id="rId71" location="/runs/details/1e5fbfec-3bf5-4ade-8545-f779670b738e" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/1e5fbfec-3bf5-4ade-8545-f779670b738e" xr:uid="{BC32C75D-72D2-8449-8092-29A3207175F9}"/>
+    <hyperlink ref="B46" r:id="rId72" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/a92ac11f-3fea-4575-b6cb-81a184d61a71" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/a92ac11f-3fea-4575-b6cb-81a184d61a71" xr:uid="{A4412B4A-E318-3943-869B-2B3E26FCB5FE}"/>
+    <hyperlink ref="A47" r:id="rId73" location="/runs/details/7cc84181-66d5-44d5-912f-d5d544e00167" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/7cc84181-66d5-44d5-912f-d5d544e00167" xr:uid="{D474C986-E3BA-C748-A623-7B30E07F4D19}"/>
+    <hyperlink ref="B47" r:id="rId74" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/e0faf63c-8fe1-4f24-b084-80cc8f354ba1" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/e0faf63c-8fe1-4f24-b084-80cc8f354ba1" xr:uid="{778DE83C-75C7-214A-99C4-D3CF79D6C6F8}"/>
+    <hyperlink ref="A48" r:id="rId75" location="/runs/details/0e9e9bc5-da6c-4ab8-9de9-89dd925ee5cc" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /runs/details/0e9e9bc5-da6c-4ab8-9de9-89dd925ee5cc" xr:uid="{52641D50-7A27-C549-B126-EA1CEF1DD22F}"/>
+    <hyperlink ref="B48" r:id="rId76" location="/pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/241db350-be5d-4c4e-bca4-ff1c54cc1cbf" display="https://df6bc4688870067-dot-us-east1.pipelines.googleusercontent.com/ - /pipelines/details/ce0d5acc-4c98-454a-ad0a-d603424d9973/version/241db350-be5d-4c4e-bca4-ff1c54cc1cbf" xr:uid="{4A5E8AA6-9A5D-3842-B4EF-C7F5D05C110A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>